<commit_message>
Clean up for evaluation
</commit_message>
<xml_diff>
--- a/figures/Results Paper.xlsx
+++ b/figures/Results Paper.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Udo\Documents\Documents_Sync\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Udo\git\ts-mule\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="13310" windowHeight="120"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="13305" windowHeight="120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$64</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$67</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -484,22 +484,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G62"/>
+  <dimension ref="B2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6328125" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
-    <col min="3" max="4" width="17.54296875" customWidth="1"/>
-    <col min="5" max="5" width="19.6328125" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -519,7 +519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -537,10 +537,10 @@
       </c>
       <c r="G3" t="str">
         <f>E3&amp;" &amp; "&amp;D3&amp;" &amp; "&amp;C3</f>
-        <v>1.31 &amp; 2.11 &amp; 1.95</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+        <v>1,31 &amp; 2,11 &amp; 1,95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="1">
         <v>2.2999999999999998</v>
@@ -554,8 +554,12 @@
       <c r="F4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G4" t="str">
+        <f>E4&amp;" &amp; "&amp;D4&amp;" &amp; "&amp;C4</f>
+        <v>1,15 &amp; 2,66 &amp; 2,3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="C5" s="8">
         <v>2.64</v>
@@ -569,916 +573,1074 @@
       <c r="F5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
+      <c r="G5" t="str">
+        <f>E5&amp;" &amp; "&amp;D5&amp;" &amp; "&amp;C5</f>
+        <v>0,19 &amp; 4,35 &amp; 2,64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C9" s="3">
         <v>3.6</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D9" s="3">
         <v>3.43</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E9" s="4">
         <v>0.35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="str">
-        <f>E6&amp;" &amp; "&amp;D6&amp;" &amp; "&amp;C6</f>
-        <v>0.35 &amp; 3.43 &amp; 3.6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
-      <c r="C7" s="1">
-        <v>5.22</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0.46</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8">
-        <v>3.25</v>
-      </c>
-      <c r="D8" s="8">
-        <v>10.06</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0.23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2.38</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.22</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.69</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
       </c>
       <c r="G9" t="str">
         <f>E9&amp;" &amp; "&amp;D9&amp;" &amp; "&amp;C9</f>
-        <v>1.69 &amp; 1.22 &amp; 2.38</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+        <v>0,35 &amp; 3,43 &amp; 3,6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="1">
-        <v>2.02</v>
+        <v>5.22</v>
       </c>
       <c r="D10" s="1">
-        <v>1.1100000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="E10" s="6">
-        <v>1.72</v>
+        <v>0.46</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G10" t="str">
+        <f>E10&amp;" &amp; "&amp;D10&amp;" &amp; "&amp;C10</f>
+        <v>0,46 &amp; 4,2 &amp; 5,22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="8">
-        <v>1.63</v>
+        <v>3.25</v>
       </c>
       <c r="D11" s="8">
-        <v>3.13</v>
+        <v>10.06</v>
       </c>
       <c r="E11" s="9">
-        <v>2.67</v>
+        <v>0.23</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G11" t="str">
+        <f>E11&amp;" &amp; "&amp;D11&amp;" &amp; "&amp;C11</f>
+        <v>0,23 &amp; 10,06 &amp; 3,25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3">
-        <v>2.3199999999999998</v>
+        <v>2.38</v>
       </c>
       <c r="D12" s="3">
-        <v>4.24</v>
+        <v>1.22</v>
       </c>
       <c r="E12" s="4">
-        <v>2.31</v>
+        <v>1.69</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="str">
         <f>E12&amp;" &amp; "&amp;D12&amp;" &amp; "&amp;C12</f>
-        <v>2.31 &amp; 4.24 &amp; 2.32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+        <v>1,69 &amp; 1,22 &amp; 2,38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="1">
-        <v>2.04</v>
+        <v>2.02</v>
       </c>
       <c r="D13" s="1">
-        <v>3.92</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="E13" s="6">
-        <v>2.2200000000000002</v>
+        <v>1.72</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G13" t="str">
+        <f>E13&amp;" &amp; "&amp;D13&amp;" &amp; "&amp;C13</f>
+        <v>1,72 &amp; 1,11 &amp; 2,02</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="8">
-        <v>2.64</v>
+        <v>1.63</v>
       </c>
       <c r="D14" s="8">
-        <v>4.0999999999999996</v>
+        <v>3.13</v>
       </c>
       <c r="E14" s="9">
-        <v>1.06</v>
+        <v>2.67</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G14" t="str">
+        <f>E14&amp;" &amp; "&amp;D14&amp;" &amp; "&amp;C14</f>
+        <v>2,67 &amp; 3,13 &amp; 1,63</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3">
-        <v>1.41</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="D15" s="3">
-        <v>1.1200000000000001</v>
+        <v>4.24</v>
       </c>
       <c r="E15" s="4">
-        <v>0.56000000000000005</v>
+        <v>2.31</v>
       </c>
       <c r="F15" t="s">
         <v>11</v>
       </c>
       <c r="G15" t="str">
         <f>E15&amp;" &amp; "&amp;D15&amp;" &amp; "&amp;C15</f>
-        <v>0.56 &amp; 1.12 &amp; 1.41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+        <v>2,31 &amp; 4,24 &amp; 2,32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="1">
-        <v>1.98</v>
+        <v>2.04</v>
       </c>
       <c r="D16" s="1">
-        <v>1.01</v>
+        <v>3.92</v>
       </c>
       <c r="E16" s="6">
-        <v>0.66</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G16" t="str">
+        <f>E16&amp;" &amp; "&amp;D16&amp;" &amp; "&amp;C16</f>
+        <v>2,22 &amp; 3,92 &amp; 2,04</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="8">
-        <v>0.95</v>
+        <v>2.64</v>
       </c>
       <c r="D17" s="8">
-        <v>0.11</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E17" s="9">
-        <v>0.52</v>
+        <v>1.06</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G17" t="str">
+        <f>E17&amp;" &amp; "&amp;D17&amp;" &amp; "&amp;C17</f>
+        <v>1,06 &amp; 4,1 &amp; 2,64</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3">
-        <v>2.23</v>
+        <v>1.41</v>
       </c>
       <c r="D18" s="3">
-        <v>2.58</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E18" s="4">
-        <v>1.24</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
       </c>
       <c r="G18" t="str">
         <f>E18&amp;" &amp; "&amp;D18&amp;" &amp; "&amp;C18</f>
-        <v>1.24 &amp; 2.58 &amp; 2.23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+        <v>0,56 &amp; 1,12 &amp; 1,41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="1">
-        <v>2.61</v>
+        <v>1.98</v>
       </c>
       <c r="D19" s="1">
-        <v>2.92</v>
+        <v>1.01</v>
       </c>
       <c r="E19" s="6">
-        <v>1.23</v>
+        <v>0.66</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G19" t="str">
+        <f>E19&amp;" &amp; "&amp;D19&amp;" &amp; "&amp;C19</f>
+        <v>0,66 &amp; 1,01 &amp; 1,98</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="8">
-        <v>2.1800000000000002</v>
+        <v>0.95</v>
       </c>
       <c r="D20" s="8">
-        <v>4.25</v>
+        <v>0.11</v>
       </c>
       <c r="E20" s="9">
-        <v>0.78</v>
+        <v>0.52</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" t="s">
+      <c r="G20" t="str">
+        <f>E20&amp;" &amp; "&amp;D20&amp;" &amp; "&amp;C20</f>
+        <v>0,52 &amp; 0,11 &amp; 0,95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2.23</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2.58</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="str">
+        <f>E21&amp;" &amp; "&amp;D21&amp;" &amp; "&amp;C21</f>
+        <v>1,24 &amp; 2,58 &amp; 2,23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="1">
+        <v>2.61</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2.92</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1.23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="str">
+        <f>E22&amp;" &amp; "&amp;D22&amp;" &amp; "&amp;C22</f>
+        <v>1,23 &amp; 2,92 &amp; 2,61</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D23" s="8">
+        <v>4.25</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.78</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="str">
+        <f>E23&amp;" &amp; "&amp;D23&amp;" &amp; "&amp;C23</f>
+        <v>0,78 &amp; 4,25 &amp; 2,18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>0</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>2</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>8</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>9</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F26" t="s">
         <v>14</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="2" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C27" s="3">
         <v>3.97</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D27" s="3">
         <v>6.76</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E27" s="4">
         <v>1.3</v>
-      </c>
-      <c r="F24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" t="str">
-        <f>E24&amp;" &amp; "&amp;D24&amp;" &amp; "&amp;C24</f>
-        <v>1.3 &amp; 6.76 &amp; 3.97</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="5"/>
-      <c r="C25" s="1">
-        <v>5.79</v>
-      </c>
-      <c r="D25" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E25" s="6">
-        <v>1.59</v>
-      </c>
-      <c r="F25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="7"/>
-      <c r="C26" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="D26" s="8">
-        <v>-4.9000000000000004</v>
-      </c>
-      <c r="E26" s="9">
-        <v>14.53</v>
-      </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="3">
-        <v>5.71</v>
-      </c>
-      <c r="D27" s="3">
-        <v>10.46</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0.41</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
       </c>
       <c r="G27" t="str">
         <f>E27&amp;" &amp; "&amp;D27&amp;" &amp; "&amp;C27</f>
-        <v>0.41 &amp; 10.46 &amp; 5.71</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+        <v>1,3 &amp; 6,76 &amp; 3,97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="1">
-        <v>4.3499999999999996</v>
+        <v>5.79</v>
       </c>
       <c r="D28" s="1">
-        <v>7.41</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E28" s="6">
-        <v>0.37</v>
+        <v>1.59</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G28" t="str">
+        <f>E28&amp;" &amp; "&amp;D28&amp;" &amp; "&amp;C28</f>
+        <v>1,59 &amp; 4,1 &amp; 5,79</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="8">
-        <v>1.07</v>
+        <v>1.2</v>
       </c>
       <c r="D29" s="8">
-        <v>14.9</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="E29" s="9">
-        <v>0.81</v>
+        <v>14.53</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G29" t="str">
+        <f>E29&amp;" &amp; "&amp;D29&amp;" &amp; "&amp;C29</f>
+        <v>14,53 &amp; -4,9 &amp; 1,2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3">
-        <v>2.67</v>
+        <v>5.71</v>
       </c>
       <c r="D30" s="3">
-        <v>1.68</v>
+        <v>10.46</v>
       </c>
       <c r="E30" s="4">
-        <v>1.52</v>
+        <v>0.41</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
       </c>
       <c r="G30" t="str">
         <f>E30&amp;" &amp; "&amp;D30&amp;" &amp; "&amp;C30</f>
-        <v>1.52 &amp; 1.68 &amp; 2.67</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+        <v>0,41 &amp; 10,46 &amp; 5,71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="1">
-        <v>5.37</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="D31" s="1">
-        <v>1.6</v>
+        <v>7.41</v>
       </c>
       <c r="E31" s="6">
-        <v>1.48</v>
+        <v>0.37</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G31" t="str">
+        <f>E31&amp;" &amp; "&amp;D31&amp;" &amp; "&amp;C31</f>
+        <v>0,37 &amp; 7,41 &amp; 4,35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="8">
         <v>1.07</v>
       </c>
       <c r="D32" s="8">
-        <v>2.9</v>
+        <v>14.9</v>
       </c>
       <c r="E32" s="9">
-        <v>51.33</v>
+        <v>0.81</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G32" t="str">
+        <f>E32&amp;" &amp; "&amp;D32&amp;" &amp; "&amp;C32</f>
+        <v>0,81 &amp; 14,9 &amp; 1,07</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C33" s="3">
-        <v>7.67</v>
+        <v>2.67</v>
       </c>
       <c r="D33" s="3">
-        <v>9</v>
+        <v>1.68</v>
       </c>
       <c r="E33" s="4">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
       </c>
       <c r="G33" t="str">
         <f>E33&amp;" &amp; "&amp;D33&amp;" &amp; "&amp;C33</f>
-        <v>1.5 &amp; 9 &amp; 7.67</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+        <v>1,52 &amp; 1,68 &amp; 2,67</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="1">
-        <v>6.27</v>
+        <v>5.37</v>
       </c>
       <c r="D34" s="1">
         <v>1.6</v>
       </c>
       <c r="E34" s="6">
-        <v>1.67</v>
+        <v>1.48</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G34" t="str">
+        <f>E34&amp;" &amp; "&amp;D34&amp;" &amp; "&amp;C34</f>
+        <v>1,48 &amp; 1,6 &amp; 5,37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="7"/>
       <c r="C35" s="8">
-        <v>1.0900000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="D35" s="8">
-        <v>2.89</v>
+        <v>2.9</v>
       </c>
       <c r="E35" s="9">
-        <v>3.7</v>
+        <v>51.33</v>
       </c>
       <c r="F35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G35" t="str">
+        <f>E35&amp;" &amp; "&amp;D35&amp;" &amp; "&amp;C35</f>
+        <v>51,33 &amp; 2,9 &amp; 1,07</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" s="3">
-        <v>11.52</v>
+        <v>7.67</v>
       </c>
       <c r="D36" s="3">
-        <v>0.16</v>
+        <v>9</v>
       </c>
       <c r="E36" s="4">
-        <v>0.62</v>
+        <v>1.5</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
       </c>
       <c r="G36" t="str">
         <f>E36&amp;" &amp; "&amp;D36&amp;" &amp; "&amp;C36</f>
-        <v>0.62 &amp; 0.16 &amp; 11.52</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+        <v>1,5 &amp; 9 &amp; 7,67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="C37" s="1">
-        <v>9.2799999999999994</v>
+        <v>6.27</v>
       </c>
       <c r="D37" s="1">
-        <v>0.11</v>
+        <v>1.6</v>
       </c>
       <c r="E37" s="6">
-        <v>0.65</v>
+        <v>1.67</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G37" t="str">
+        <f>E37&amp;" &amp; "&amp;D37&amp;" &amp; "&amp;C37</f>
+        <v>1,67 &amp; 1,6 &amp; 6,27</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="8">
-        <v>1</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="D38" s="8">
-        <v>-0.04</v>
+        <v>2.89</v>
       </c>
       <c r="E38" s="9">
-        <v>0.78</v>
+        <v>3.7</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G38" t="str">
+        <f>E38&amp;" &amp; "&amp;D38&amp;" &amp; "&amp;C38</f>
+        <v>3,7 &amp; 2,89 &amp; 1,09</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C39" s="3">
-        <v>4.1500000000000004</v>
+        <v>11.52</v>
       </c>
       <c r="D39" s="3">
-        <v>8</v>
+        <v>0.16</v>
       </c>
       <c r="E39" s="4">
-        <v>1.1000000000000001</v>
+        <v>0.62</v>
       </c>
       <c r="F39" t="s">
         <v>11</v>
       </c>
       <c r="G39" t="str">
         <f>E39&amp;" &amp; "&amp;D39&amp;" &amp; "&amp;C39</f>
-        <v>1.1 &amp; 8 &amp; 4.15</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+        <v>0,62 &amp; 0,16 &amp; 11,52</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="1">
-        <v>4.3</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="D40" s="1">
-        <v>5.89</v>
+        <v>0.11</v>
       </c>
       <c r="E40" s="6">
-        <v>2.04</v>
+        <v>0.65</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G40" t="str">
+        <f>E40&amp;" &amp; "&amp;D40&amp;" &amp; "&amp;C40</f>
+        <v>0,65 &amp; 0,11 &amp; 9,28</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="8">
-        <v>2.91</v>
+        <v>1</v>
       </c>
       <c r="D41" s="8">
-        <v>5.0599999999999996</v>
+        <v>-0.04</v>
       </c>
       <c r="E41" s="9">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" t="s">
+      <c r="G41" t="str">
+        <f>E41&amp;" &amp; "&amp;D41&amp;" &amp; "&amp;C41</f>
+        <v>0,78 &amp; -0,04 &amp; 1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="3">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="D42" s="3">
+        <v>8</v>
+      </c>
+      <c r="E42" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="str">
+        <f>E42&amp;" &amp; "&amp;D42&amp;" &amp; "&amp;C42</f>
+        <v>1,1 &amp; 8 &amp; 4,15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="D43" s="1">
+        <v>5.89</v>
+      </c>
+      <c r="E43" s="6">
+        <v>2.04</v>
+      </c>
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" t="str">
+        <f>E43&amp;" &amp; "&amp;D43&amp;" &amp; "&amp;C43</f>
+        <v>2,04 &amp; 5,89 &amp; 4,3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="7"/>
+      <c r="C44" s="8">
+        <v>2.91</v>
+      </c>
+      <c r="D44" s="8">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0.76</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" t="str">
+        <f>E44&amp;" &amp; "&amp;D44&amp;" &amp; "&amp;C44</f>
+        <v>0,76 &amp; 5,06 &amp; 2,91</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>10</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" t="s">
         <v>2</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D47" t="s">
         <v>8</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E47" t="s">
         <v>9</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F47" t="s">
         <v>14</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B45" s="2" t="s">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C48" s="3">
         <v>9.2899999999999991</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D48" s="3">
         <v>-0.18</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E48" s="4">
         <v>3.39</v>
-      </c>
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" t="str">
-        <f>E45&amp;" &amp; "&amp;D45&amp;" &amp; "&amp;C45</f>
-        <v>3.39 &amp; -0.18 &amp; 9.29</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B46" s="5"/>
-      <c r="C46" s="1">
-        <v>6.14</v>
-      </c>
-      <c r="D46" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="E46" s="6">
-        <v>2.37</v>
-      </c>
-      <c r="F46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="7"/>
-      <c r="C47" s="8">
-        <v>6.36</v>
-      </c>
-      <c r="D47" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="E47" s="9">
-        <v>1.21</v>
-      </c>
-      <c r="F47" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="3">
-        <v>7.38</v>
-      </c>
-      <c r="D48" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="E48" s="4">
-        <v>1.25</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
       </c>
       <c r="G48" t="str">
         <f>E48&amp;" &amp; "&amp;D48&amp;" &amp; "&amp;C48</f>
-        <v>1.25 &amp; 0.4 &amp; 7.38</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+        <v>3,39 &amp; -0,18 &amp; 9,29</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="1">
-        <v>3.99</v>
+        <v>6.14</v>
       </c>
       <c r="D49" s="1">
-        <v>0.49</v>
+        <v>0.12</v>
       </c>
       <c r="E49" s="6">
-        <v>1</v>
+        <v>2.37</v>
       </c>
       <c r="F49" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G49" t="str">
+        <f>E49&amp;" &amp; "&amp;D49&amp;" &amp; "&amp;C49</f>
+        <v>2,37 &amp; 0,12 &amp; 6,14</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="8">
-        <v>6.18</v>
+        <v>6.36</v>
       </c>
       <c r="D50" s="8">
-        <v>0.35</v>
+        <v>0.8</v>
       </c>
       <c r="E50" s="9">
-        <v>2.5499999999999998</v>
+        <v>1.21</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G50" t="str">
+        <f>E50&amp;" &amp; "&amp;D50&amp;" &amp; "&amp;C50</f>
+        <v>1,21 &amp; 0,8 &amp; 6,36</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" s="3">
-        <v>2.68</v>
+        <v>7.38</v>
       </c>
       <c r="D51" s="3">
-        <v>0.44</v>
+        <v>0.4</v>
       </c>
       <c r="E51" s="4">
-        <v>1.44</v>
+        <v>1.25</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
       </c>
       <c r="G51" t="str">
         <f>E51&amp;" &amp; "&amp;D51&amp;" &amp; "&amp;C51</f>
-        <v>1.44 &amp; 0.44 &amp; 2.68</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+        <v>1,25 &amp; 0,4 &amp; 7,38</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="1">
-        <v>1.65</v>
+        <v>3.99</v>
       </c>
       <c r="D52" s="1">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="E52" s="6">
-        <v>1.17</v>
+        <v>1</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G52" t="str">
+        <f>E52&amp;" &amp; "&amp;D52&amp;" &amp; "&amp;C52</f>
+        <v>1 &amp; 0,49 &amp; 3,99</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="7"/>
       <c r="C53" s="8">
-        <v>4.04</v>
+        <v>6.18</v>
       </c>
       <c r="D53" s="8">
-        <v>0.9</v>
+        <v>0.35</v>
       </c>
       <c r="E53" s="9">
-        <v>1.56</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F53" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G53" t="str">
+        <f>E53&amp;" &amp; "&amp;D53&amp;" &amp; "&amp;C53</f>
+        <v>2,55 &amp; 0,35 &amp; 6,18</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C54" s="3">
-        <v>6.55</v>
+        <v>2.68</v>
       </c>
       <c r="D54" s="3">
-        <v>-0.22</v>
+        <v>0.44</v>
       </c>
       <c r="E54" s="4">
-        <v>2.4300000000000002</v>
+        <v>1.44</v>
       </c>
       <c r="F54" t="s">
         <v>11</v>
       </c>
       <c r="G54" t="str">
         <f>E54&amp;" &amp; "&amp;D54&amp;" &amp; "&amp;C54</f>
-        <v>2.43 &amp; -0.22 &amp; 6.55</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+        <v>1,44 &amp; 0,44 &amp; 2,68</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="1">
-        <v>3.98</v>
+        <v>1.65</v>
       </c>
       <c r="D55" s="1">
-        <v>-0.28999999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="E55" s="6">
-        <v>1.9</v>
+        <v>1.17</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G55" t="str">
+        <f>E55&amp;" &amp; "&amp;D55&amp;" &amp; "&amp;C55</f>
+        <v>1,17 &amp; 0,5 &amp; 1,65</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="8">
-        <v>4.43</v>
+        <v>4.04</v>
       </c>
       <c r="D56" s="8">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E56" s="9">
-        <v>1.1100000000000001</v>
+        <v>1.56</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G56" t="str">
+        <f>E56&amp;" &amp; "&amp;D56&amp;" &amp; "&amp;C56</f>
+        <v>1,56 &amp; 0,9 &amp; 4,04</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57" s="3">
-        <v>0.62</v>
+        <v>6.55</v>
       </c>
       <c r="D57" s="3">
-        <v>-0.01</v>
+        <v>-0.22</v>
       </c>
       <c r="E57" s="4">
-        <v>0.55000000000000004</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="F57" t="s">
         <v>11</v>
       </c>
       <c r="G57" t="str">
         <f>E57&amp;" &amp; "&amp;D57&amp;" &amp; "&amp;C57</f>
-        <v>0.55 &amp; -0.01 &amp; 0.62</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
+        <v>2,43 &amp; -0,22 &amp; 6,55</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="1">
-        <v>0.59</v>
+        <v>3.98</v>
       </c>
       <c r="D58" s="1">
-        <v>-0.02</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="E58" s="6">
-        <v>0.54</v>
+        <v>1.9</v>
       </c>
       <c r="F58" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G58" t="str">
+        <f>E58&amp;" &amp; "&amp;D58&amp;" &amp; "&amp;C58</f>
+        <v>1,9 &amp; -0,29 &amp; 3,98</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="7"/>
       <c r="C59" s="8">
-        <v>0.45</v>
+        <v>4.43</v>
       </c>
       <c r="D59" s="8">
-        <v>-0.03</v>
+        <v>0.26</v>
       </c>
       <c r="E59" s="9">
-        <v>0.65</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="F59" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G59" t="str">
+        <f>E59&amp;" &amp; "&amp;D59&amp;" &amp; "&amp;C59</f>
+        <v>1,11 &amp; 0,26 &amp; 4,43</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C60" s="3">
-        <v>7.34</v>
+        <v>0.62</v>
       </c>
       <c r="D60" s="3">
-        <v>-1.1599999999999999</v>
+        <v>-0.01</v>
       </c>
       <c r="E60" s="4">
-        <v>1.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F60" t="s">
         <v>11</v>
       </c>
       <c r="G60" t="str">
         <f>E60&amp;" &amp; "&amp;D60&amp;" &amp; "&amp;C60</f>
-        <v>1.55 &amp; -1.16 &amp; 7.34</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
+        <v>0,55 &amp; -0,01 &amp; 0,62</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="1">
-        <v>4.8099999999999996</v>
+        <v>0.59</v>
       </c>
       <c r="D61" s="1">
-        <v>-1.01</v>
+        <v>-0.02</v>
       </c>
       <c r="E61" s="6">
-        <v>1.23</v>
+        <v>0.54</v>
       </c>
       <c r="F61" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G61" t="str">
+        <f>E61&amp;" &amp; "&amp;D61&amp;" &amp; "&amp;C61</f>
+        <v>0,54 &amp; -0,02 &amp; 0,59</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="7"/>
       <c r="C62" s="8">
-        <v>4.1399999999999997</v>
+        <v>0.45</v>
       </c>
       <c r="D62" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>-0.03</v>
       </c>
       <c r="E62" s="9">
-        <v>1.73</v>
+        <v>0.65</v>
       </c>
       <c r="F62" t="s">
         <v>13</v>
       </c>
+      <c r="G62" t="str">
+        <f>E62&amp;" &amp; "&amp;D62&amp;" &amp; "&amp;C62</f>
+        <v>0,65 &amp; -0,03 &amp; 0,45</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="3">
+        <v>7.34</v>
+      </c>
+      <c r="D63" s="3">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="E63" s="4">
+        <v>1.55</v>
+      </c>
+      <c r="F63" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" t="str">
+        <f>E63&amp;" &amp; "&amp;D63&amp;" &amp; "&amp;C63</f>
+        <v>1,55 &amp; -1,16 &amp; 7,34</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="C64" s="1">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="D64" s="1">
+        <v>-1.01</v>
+      </c>
+      <c r="E64" s="6">
+        <v>1.23</v>
+      </c>
+      <c r="F64" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" t="str">
+        <f>E64&amp;" &amp; "&amp;D64&amp;" &amp; "&amp;C64</f>
+        <v>1,23 &amp; -1,01 &amp; 4,81</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="7"/>
+      <c r="C65" s="8">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="D65" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E65" s="9">
+        <v>1.73</v>
+      </c>
+      <c r="F65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" t="str">
+        <f>E65&amp;" &amp; "&amp;D65&amp;" &amp; "&amp;C65</f>
+        <v>1,73 &amp; 0,07 &amp; 4,14</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C45 C48 C51 C54 C57">
+  <conditionalFormatting sqref="C48 C51 C54 C57 C60">
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
@@ -1490,7 +1652,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45 D48 D51 D54 D57">
+  <conditionalFormatting sqref="D48 D51 D54 D57 D60">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
@@ -1502,7 +1664,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45 E48 E51 E54 E57">
+  <conditionalFormatting sqref="E48 E51 E54 E57 E60">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -1514,7 +1676,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46 C49 C52 C55 C58">
+  <conditionalFormatting sqref="C49 C52 C55 C58 C61">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -1526,7 +1688,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46 D49 D52 D55 D58">
+  <conditionalFormatting sqref="D49 D52 D55 D58 D61">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -1538,7 +1700,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46 E49 E52 E55 E58">
+  <conditionalFormatting sqref="E49 E52 E55 E58 E61">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -1550,7 +1712,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C47 C53 C56 C59">
+  <conditionalFormatting sqref="C53 C50 C56 C59 C62">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -1562,7 +1724,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50 D47 D53 D56 D59">
+  <conditionalFormatting sqref="D53 D50 D56 D59 D62">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
@@ -1574,7 +1736,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50 E47 E53 E56 E59">
+  <conditionalFormatting sqref="E53 E50 E56 E59 E62">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -1586,7 +1748,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24 C27 C30 C33 C36">
+  <conditionalFormatting sqref="C27 C30 C33 C36 C39">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -1598,7 +1760,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25 C28 C31 C34 C37">
+  <conditionalFormatting sqref="C28 C31 C34 C37 C40">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -1610,7 +1772,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26 C29 C32 C35 C38">
+  <conditionalFormatting sqref="C29 C32 C35 C38 C41">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -1622,7 +1784,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24 D27 D30 D33 D36">
+  <conditionalFormatting sqref="D27 D30 D33 D36 D39">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -1634,7 +1796,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25 D28 D31 D34 D37">
+  <conditionalFormatting sqref="D28 D31 D34 D37 D40">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -1646,7 +1808,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26 D29 D32 D35 D38">
+  <conditionalFormatting sqref="D29 D32 D35 D38 D41">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -1658,7 +1820,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24 E27 E30 E33 E36">
+  <conditionalFormatting sqref="E27 E30 E33 E36 E39">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -1670,7 +1832,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25 E28 E31 E34 E37">
+  <conditionalFormatting sqref="E28 E31 E34 E37 E40">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -1682,7 +1844,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26 E29 E32 E35 E38">
+  <conditionalFormatting sqref="E29 E32 E35 E38 E41">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -1694,7 +1856,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3 C6 C9 C12 C15">
+  <conditionalFormatting sqref="C3 C9 C12 C15 C18">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -1706,7 +1868,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4 C7 C10 C13 C16">
+  <conditionalFormatting sqref="C4 C10 C13 C16 C19">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -1718,7 +1880,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5 C8 C11 C14 C17">
+  <conditionalFormatting sqref="C5:C8 C11 C14 C17 C20">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -1730,7 +1892,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3 D6 D9 D12 D15">
+  <conditionalFormatting sqref="D3 D9 D12 D15 D18">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -1742,7 +1904,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 D7 D10 D13 D16">
+  <conditionalFormatting sqref="D4 D10 D13 D16 D19">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -1754,7 +1916,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5 D8 D11 D14 D17">
+  <conditionalFormatting sqref="D5:D8 D11 D14 D17 D20">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -1766,7 +1928,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3 E6 E9 E12 E15">
+  <conditionalFormatting sqref="E3 E9 E12 E15 E18">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -1778,7 +1940,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 E7 E10 E13 E16">
+  <conditionalFormatting sqref="E4 E10 E13 E16 E19">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -1790,7 +1952,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5 E8 E11 E14 E17">
+  <conditionalFormatting sqref="E5:E8 E11 E14 E17 E20">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -1802,7 +1964,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36 C39 C33 C30 C27 C24">
+  <conditionalFormatting sqref="C39 C42 C36 C33 C30 C27">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -1814,7 +1976,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37 C40 C34 C31 C28 C25">
+  <conditionalFormatting sqref="C40 C43 C37 C34 C31 C28">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -1826,7 +1988,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38 C41 C35 C32 C29 C26">
+  <conditionalFormatting sqref="C41 C44 C38 C35 C32 C29">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -1838,7 +2000,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24 D27 D30 D33 D36 D39">
+  <conditionalFormatting sqref="D27 D30 D33 D36 D39 D42">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -1850,7 +2012,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37 D40 D34 D31 D25 D28">
+  <conditionalFormatting sqref="D40 D43 D37 D34 D28 D31">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -1862,7 +2024,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38 D41 D35 D32 D29 D26">
+  <conditionalFormatting sqref="D41 D44 D38 D35 D32 D29">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -1874,7 +2036,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36 E39 E33 E30 E27 E24">
+  <conditionalFormatting sqref="E39 E42 E36 E33 E30 E27">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -1886,7 +2048,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37 E40 E34 E31 E28 E25">
+  <conditionalFormatting sqref="E40 E43 E37 E34 E31 E28">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -1898,7 +2060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35 E38 E41 E32 E29 E26">
+  <conditionalFormatting sqref="E38 E41 E44 E35 E32 E29">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -1910,7 +2072,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15 C18 C12 C9 C6 C3">
+  <conditionalFormatting sqref="C18 C21 C15 C12 C9 C3">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -1922,7 +2084,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15 C18 C12 C9 C6 C3">
+  <conditionalFormatting sqref="C18 C21 C15 C12 C9 C3">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -1934,7 +2096,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4 C8 C10 C13 C16 C19">
+  <conditionalFormatting sqref="C4 C11 C13 C16 C19 C22">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -1946,7 +2108,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4 C7 C10 C13 C16 C19">
+  <conditionalFormatting sqref="C4 C10 C13 C16 C19 C22">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -1958,7 +2120,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5 C8 C11 C14 C17 C20">
+  <conditionalFormatting sqref="C5:C8 C11 C14 C17 C20 C23">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -1970,7 +2132,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3 D6 D9 D12 D15 D18">
+  <conditionalFormatting sqref="D3 D9 D12 D15 D18 D21">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -1982,7 +2144,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 D10 D4 D13 D16 D19">
+  <conditionalFormatting sqref="D10 D13 D4 D16 D19 D22">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -1994,7 +2156,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5 D8 D11 D14 D17 D20">
+  <conditionalFormatting sqref="D5:D8 D11 D14 D17 D20 D23">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2006,7 +2168,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3 E6 E9 E12 E15 E18">
+  <conditionalFormatting sqref="E3 E9 E12 E15 E18 E21">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -2030,7 +2192,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 E7 E10 E13 E16 E19">
+  <conditionalFormatting sqref="E4 E10 E13 E16 E19 E22">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2042,7 +2204,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5 E8 E11 E14 E17 E20">
+  <conditionalFormatting sqref="E5:E8 E11 E14 E17 E20 E23">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2054,7 +2216,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24 C27 C30 C33 C36 C39">
+  <conditionalFormatting sqref="C27 C30 C33 C36 C39 C42">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2066,7 +2228,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25 C28 C31 C34 C37 C40">
+  <conditionalFormatting sqref="C28 C31 C34 C37 C40 C43">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -2078,7 +2240,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26 C29 C32 C35 C38 C41">
+  <conditionalFormatting sqref="C29 C32 C35 C38 C41 C44">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2090,7 +2252,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24 D27 D30 D33 D36 D39">
+  <conditionalFormatting sqref="D27 D30 D33 D36 D39 D42">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2102,7 +2264,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25 D28 D31 D34 D37 D40">
+  <conditionalFormatting sqref="D28 D31 D34 D37 D40 D43">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2114,7 +2276,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26 D29 D32 D35 D38 D41">
+  <conditionalFormatting sqref="D29 D32 D35 D38 D41 D44">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2126,7 +2288,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24 E27 E30 E33 E36 E39">
+  <conditionalFormatting sqref="E27 E30 E33 E36 E39 E42">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2138,7 +2300,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25 E28 E31 E34 E37 E40">
+  <conditionalFormatting sqref="E28 E31 E34 E37 E40 E43">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2150,7 +2312,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26 E29 E32 E35 E38 E41">
+  <conditionalFormatting sqref="E29 E32 E35 E38 E41 E44">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2162,7 +2324,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45 C48 C51 C54 C57 C60">
+  <conditionalFormatting sqref="C48 C51 C54 C57 C60 C63">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2174,7 +2336,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46 C49 C52 C55 C58 C61">
+  <conditionalFormatting sqref="C49 C52 C55 C58 C61 C64">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2186,7 +2348,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C47 C53 C56 C59 C62">
+  <conditionalFormatting sqref="C53 C50 C56 C59 C62 C65">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2198,7 +2360,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45 D48 D51 D54 D57 D60">
+  <conditionalFormatting sqref="D48 D51 D54 D57 D60 D63">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2210,7 +2372,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46 D49 D52 D55 D58 D61">
+  <conditionalFormatting sqref="D49 D52 D55 D58 D61 D64">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2222,7 +2384,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50 D47 D53 D56 D59 D62">
+  <conditionalFormatting sqref="D53 D50 D56 D59 D62 D65">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2234,7 +2396,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45 E48 E51 E54 E57 E60">
+  <conditionalFormatting sqref="E48 E51 E54 E57 E60 E63">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2246,7 +2408,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46 E49 E52 E55 E58 E61">
+  <conditionalFormatting sqref="E49 E52 E55 E58 E61 E64">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2258,7 +2420,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50 E47 E53 E56 E59 E62">
+  <conditionalFormatting sqref="E53 E50 E56 E59 E62 E65">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>